<commit_message>
summary the exp 1
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\MTVAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64FEFB4-CBE6-488F-BCAC-2E11054EA000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D06ABF-9004-4847-844A-E2EA0C3FA505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="exp1(100net)" sheetId="3" r:id="rId1"/>
+    <sheet name="network(BDE)" sheetId="3" r:id="rId1"/>
+    <sheet name="Rec(A)" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
   <si>
     <t>β0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -128,6 +129,18 @@
   </si>
   <si>
     <t>Fake (2) z=4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A. Rec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PFM (1) z=4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -295,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,31 +340,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694FA8BF-FDF9-4164-B4EA-D9FA0E639984}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.5"/>
@@ -693,15 +712,15 @@
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="14"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
@@ -710,21 +729,21 @@
       <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="13" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="14"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
@@ -733,7 +752,7 @@
       <c r="B6" s="9">
         <v>100</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -770,10 +789,10 @@
         <f t="shared" ref="E7:E11" si="0">ABS(D7-$E$2)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="11">
         <v>0.54720000000000002</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="12">
         <f t="shared" ref="G7:G11" si="1">ABS(F7-$E$2)</f>
         <v>4.720000000000002E-2</v>
       </c>
@@ -796,10 +815,10 @@
         <f t="shared" si="0"/>
         <v>0.1341</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="13">
         <v>0.56979999999999997</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="14">
         <f t="shared" si="1"/>
         <v>6.9799999999999973E-2</v>
       </c>
@@ -822,10 +841,10 @@
         <f t="shared" si="0"/>
         <v>0.19869999999999999</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="11">
         <v>0.57340000000000002</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="12">
         <f t="shared" si="1"/>
         <v>7.3400000000000021E-2</v>
       </c>
@@ -848,10 +867,10 @@
         <f t="shared" si="0"/>
         <v>0.25270000000000004</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="13">
         <v>0.57350000000000001</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="14">
         <f t="shared" si="1"/>
         <v>7.350000000000001E-2</v>
       </c>
@@ -874,10 +893,10 @@
         <f t="shared" si="0"/>
         <v>0.3024</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="11">
         <v>0.58320000000000005</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="12">
         <f t="shared" si="1"/>
         <v>8.3200000000000052E-2</v>
       </c>
@@ -896,15 +915,15 @@
       <c r="B13" s="9">
         <v>0</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="14"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" s="9" t="s">
@@ -913,21 +932,21 @@
       <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="13" t="s">
+      <c r="E14" s="16"/>
+      <c r="F14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="13" t="s">
+      <c r="G14" s="16"/>
+      <c r="H14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="14"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="9" t="s">
@@ -936,7 +955,7 @@
       <c r="B15" s="9">
         <v>0.4</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
@@ -973,10 +992,10 @@
         <f t="shared" ref="E16:E20" si="3">ABS(D16-$E$2)</f>
         <v>0.12060000000000004</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="11">
         <v>0.58689999999999998</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="12">
         <f t="shared" ref="G16:G20" si="4">ABS(F16-$E$2)</f>
         <v>8.6899999999999977E-2</v>
       </c>
@@ -1005,10 +1024,10 @@
         <f t="shared" si="3"/>
         <v>0.21719999999999995</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="13">
         <v>0.61370000000000002</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="14">
         <f t="shared" si="4"/>
         <v>0.11370000000000002</v>
       </c>
@@ -1031,10 +1050,10 @@
         <f t="shared" si="3"/>
         <v>0.30610000000000004</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="11">
         <v>0.61919999999999997</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="12">
         <f t="shared" si="4"/>
         <v>0.11919999999999997</v>
       </c>
@@ -1057,10 +1076,10 @@
         <f t="shared" si="3"/>
         <v>0.37529999999999997</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="13">
         <v>0.6149</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="14">
         <f t="shared" si="4"/>
         <v>0.1149</v>
       </c>
@@ -1083,10 +1102,10 @@
         <f t="shared" si="3"/>
         <v>0.43789999999999996</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="11">
         <v>0.61850000000000005</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="12">
         <f t="shared" si="4"/>
         <v>0.11850000000000005</v>
       </c>
@@ -1108,15 +1127,15 @@
       <c r="B22" s="9">
         <v>0</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="14"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="16"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" s="9" t="s">
@@ -1125,21 +1144,21 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="13" t="s">
+      <c r="E23" s="16"/>
+      <c r="F23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="13" t="s">
+      <c r="G23" s="16"/>
+      <c r="H23" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="14"/>
+      <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" s="9" t="s">
@@ -1148,7 +1167,7 @@
       <c r="B24" s="9">
         <v>100</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1185,10 +1204,10 @@
         <f t="shared" ref="E25:E29" si="6">ABS(D25-$E$2)</f>
         <v>0.21460000000000001</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="11">
         <v>0.69230000000000003</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="12">
         <f t="shared" ref="G25:G29" si="7">ABS(F25-$E$2)</f>
         <v>0.19230000000000003</v>
       </c>
@@ -1211,10 +1230,10 @@
         <f t="shared" si="6"/>
         <v>0.28590000000000004</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="13">
         <v>0.71340000000000003</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="14">
         <f t="shared" si="7"/>
         <v>0.21340000000000003</v>
       </c>
@@ -1237,10 +1256,10 @@
         <f t="shared" si="6"/>
         <v>0.35450000000000004</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="11">
         <v>0.71379999999999999</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G27" s="12">
         <f t="shared" si="7"/>
         <v>0.21379999999999999</v>
       </c>
@@ -1263,10 +1282,10 @@
         <f t="shared" si="6"/>
         <v>0.41190000000000004</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="13">
         <v>0.71379999999999999</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="14">
         <f t="shared" si="7"/>
         <v>0.21379999999999999</v>
       </c>
@@ -1289,10 +1308,10 @@
         <f t="shared" si="6"/>
         <v>0.46479999999999999</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="11">
         <v>0.71799999999999997</v>
       </c>
-      <c r="G29" s="17">
+      <c r="G29" s="12">
         <f t="shared" si="7"/>
         <v>0.21799999999999997</v>
       </c>
@@ -1326,4 +1345,187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733D0150-B160-415D-B281-5D177BF55A6E}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="2" width="4.34765625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="C4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="9">
+        <v>100</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="C6" s="19"/>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C7" s="20">
+        <v>30</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.49859999999999999</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" ref="E7:E11" si="0">ABS(D7-$E$2)</f>
+        <v>1.4000000000000123E-3</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.48609999999999998</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" ref="G7:G11" si="1">ABS(F7-$E$2)</f>
+        <v>1.3900000000000023E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C8" s="21">
+        <v>50</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C9" s="20">
+        <v>80</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C10" s="21">
+        <v>120</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C11" s="20">
+        <v>200</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update new experiments B3
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\MTVAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D5CFF8-30E0-4F67-9D8B-8DE4E3A3990C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5216A134-AAD6-41F8-990F-CA037080C059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="network(BI)" sheetId="8" r:id="rId1"/>
-    <sheet name="network(AC)" sheetId="6" r:id="rId2"/>
-    <sheet name="network(L)" sheetId="10" r:id="rId3"/>
-    <sheet name="network(DE)" sheetId="3" r:id="rId4"/>
-    <sheet name="network(FGJK)" sheetId="9" r:id="rId5"/>
+    <sheet name="debias" sheetId="12" r:id="rId1"/>
+    <sheet name="network(BI)" sheetId="8" r:id="rId2"/>
+    <sheet name="network(AC)" sheetId="6" r:id="rId3"/>
+    <sheet name="network(L)" sheetId="10" r:id="rId4"/>
+    <sheet name="network(DE)" sheetId="3" r:id="rId5"/>
+    <sheet name="network(FGJK)" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="127">
   <si>
     <t>β0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -492,6 +493,58 @@
   </si>
   <si>
     <t>VGAE_ABa5 (2) z=4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fake (4) z=4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fake (3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vgae (1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ba1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ba5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ba0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ba0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B. Unobserved Network Confounder (Ave Abs bias) z=4, epoch=200 (HSIC)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B. Unobserved Network Confounder (Ave Abs bias) z=4, epoch=200 (GRL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B. Unobserved Network Confounder (Ave Abs bias) z=4, epoch=1000 (GRL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B. Unobserved Network Confounder (Ave Abs bias) z=4, epoch=2000 (GRL)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ba2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -672,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -716,21 +769,6 @@
     <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -747,6 +785,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1034,11 +1120,734 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CE060C-EDFD-4A22-8191-C9BB0B42A61B}">
+  <dimension ref="A1:Q36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="2" width="4.34765625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C4" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6">
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.1477</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.1236</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.12189999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.1181</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.20660000000000001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.20669999999999999</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.14630000000000001</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.25530000000000003</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.255</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.17150000000000001</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.1827</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.2298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.30470000000000003</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.30280000000000001</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.1769</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.18210000000000001</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C12" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="6">
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3">
+        <v>7.7299999999999994E-2</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6">
+        <v>7.9600000000000004E-2</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9">
+        <v>100</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="2">
+        <v>0.1119</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.1123</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.1182</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.20660000000000001</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3">
+        <v>0.13919999999999999</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.14030000000000001</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.1396</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6">
+        <v>0.18629999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.25530000000000003</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.255</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.16009999999999999</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="2">
+        <v>0.1598</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0.16259999999999999</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0.22289999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.30470000000000003</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6">
+        <v>0.18429999999999999</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6">
+        <v>0.1701</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.16320000000000001</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0.25779999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="C20" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A22" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="9">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="6">
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:17" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="9">
+        <v>100</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.20660000000000001</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:17" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0.25530000000000003</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.255</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5">
+        <v>0.15920000000000001</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.30470000000000003</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="C30" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A31" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J31" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="9">
+        <v>3</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6">
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="E32" s="6">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="F32" s="3">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6">
+        <v>7.85E-2</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6">
+        <v>7.9600000000000004E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="9">
+        <v>100</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0.1477</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0.1236</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.12280000000000001</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5">
+        <v>0.1239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.20660000000000001</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.20669999999999999</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0.1431</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0.14280000000000001</v>
+      </c>
+      <c r="I34" s="6">
+        <v>0.1444</v>
+      </c>
+      <c r="J34" s="6">
+        <v>0.14480000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0.25530000000000003</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.255</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0.17380000000000001</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5">
+        <v>0.17319999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="C36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.30470000000000003</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.30280000000000001</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="3">
+        <v>0.18290000000000001</v>
+      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6">
+        <v>0.18459999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="C30:J30"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E06F339-5823-456C-9361-24347B2ACC56}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="A1:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.5"/>
@@ -1088,17 +1897,17 @@
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
@@ -1107,25 +1916,25 @@
       <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="15" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="K5" s="17"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
@@ -1134,7 +1943,7 @@
       <c r="B6" s="9">
         <v>100</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1338,17 +2147,17 @@
       <c r="B13" s="9">
         <v>0</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="9" t="s">
@@ -1357,25 +2166,25 @@
       <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="15" t="s">
+      <c r="E14" s="34"/>
+      <c r="F14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="15" t="s">
+      <c r="G14" s="34"/>
+      <c r="H14" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="K14" s="17"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" s="34"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="9" t="s">
@@ -1384,7 +2193,7 @@
       <c r="B15" s="9">
         <v>100</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1588,17 +2397,17 @@
       <c r="B22" s="9">
         <v>0</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="17"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="34"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="9" t="s">
@@ -1607,25 +2416,25 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="15" t="s">
+      <c r="E23" s="34"/>
+      <c r="F23" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="15" t="s">
+      <c r="G23" s="34"/>
+      <c r="H23" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="15" t="s">
+      <c r="I23" s="34"/>
+      <c r="J23" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="K23" s="17"/>
+      <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24" s="9" t="s">
@@ -1634,7 +2443,7 @@
       <c r="B24" s="9">
         <v>100</v>
       </c>
-      <c r="C24" s="19"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1838,15 +2647,15 @@
       <c r="B31" s="9">
         <v>0</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="17"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="34"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A32" s="9" t="s">
@@ -1855,21 +2664,21 @@
       <c r="B32" s="9">
         <v>2.5</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="15" t="s">
+      <c r="E32" s="34"/>
+      <c r="F32" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="15" t="s">
+      <c r="G32" s="34"/>
+      <c r="H32" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I32" s="17"/>
+      <c r="I32" s="34"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A33" s="9" t="s">
@@ -1878,7 +2687,7 @@
       <c r="B33" s="9">
         <v>0.5</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
@@ -2047,15 +2856,15 @@
       <c r="B40" s="9">
         <v>0</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="17"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="34"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A41" s="9" t="s">
@@ -2064,21 +2873,21 @@
       <c r="B41" s="9">
         <v>2</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="15" t="s">
+      <c r="E41" s="34"/>
+      <c r="F41" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G41" s="17"/>
-      <c r="H41" s="15" t="s">
+      <c r="G41" s="34"/>
+      <c r="H41" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I41" s="17"/>
+      <c r="I41" s="34"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A42" s="9" t="s">
@@ -2087,7 +2896,7 @@
       <c r="B42" s="9">
         <v>1</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="36"/>
       <c r="D42" s="1" t="s">
         <v>10</v>
       </c>
@@ -2256,15 +3065,15 @@
       <c r="B49" s="9">
         <v>0</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="17"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="34"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A50" s="9" t="s">
@@ -2273,21 +3082,21 @@
       <c r="B50" s="9">
         <v>1.5</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="17"/>
-      <c r="F50" s="15" t="s">
+      <c r="E50" s="34"/>
+      <c r="F50" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G50" s="17"/>
-      <c r="H50" s="15" t="s">
+      <c r="G50" s="34"/>
+      <c r="H50" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I50" s="17"/>
+      <c r="I50" s="34"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A51" s="9" t="s">
@@ -2296,7 +3105,7 @@
       <c r="B51" s="9">
         <v>1.5</v>
       </c>
-      <c r="C51" s="19"/>
+      <c r="C51" s="36"/>
       <c r="D51" s="1" t="s">
         <v>10</v>
       </c>
@@ -2465,15 +3274,15 @@
       <c r="B58" s="9">
         <v>0</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="17"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A59" s="9" t="s">
@@ -2482,21 +3291,21 @@
       <c r="B59" s="9">
         <v>1</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="15" t="s">
+      <c r="E59" s="34"/>
+      <c r="F59" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="15" t="s">
+      <c r="G59" s="34"/>
+      <c r="H59" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I59" s="17"/>
+      <c r="I59" s="34"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A60" s="9" t="s">
@@ -2505,7 +3314,7 @@
       <c r="B60" s="9">
         <v>2</v>
       </c>
-      <c r="C60" s="19"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="1" t="s">
         <v>10</v>
       </c>
@@ -2674,15 +3483,15 @@
       <c r="B67" s="9">
         <v>0</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C67" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="17"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="34"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A68" s="9" t="s">
@@ -2691,21 +3500,21 @@
       <c r="B68" s="9">
         <v>0.5</v>
       </c>
-      <c r="C68" s="18" t="s">
+      <c r="C68" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D68" s="15" t="s">
+      <c r="D68" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E68" s="17"/>
-      <c r="F68" s="15" t="s">
+      <c r="E68" s="34"/>
+      <c r="F68" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G68" s="17"/>
-      <c r="H68" s="15" t="s">
+      <c r="G68" s="34"/>
+      <c r="H68" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I68" s="17"/>
+      <c r="I68" s="34"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A69" s="9" t="s">
@@ -2714,7 +3523,7 @@
       <c r="B69" s="9">
         <v>2.5</v>
       </c>
-      <c r="C69" s="19"/>
+      <c r="C69" s="36"/>
       <c r="D69" s="1" t="s">
         <v>10</v>
       </c>
@@ -2889,38 +3698,38 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
     <mergeCell ref="C67:I67"/>
     <mergeCell ref="C68:C69"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="F68:G68"/>
     <mergeCell ref="H68:I68"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C58:I58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="C49:I49"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="F50:G50"/>
     <mergeCell ref="H50:I50"/>
     <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C49:I49"/>
     <mergeCell ref="C31:I31"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="H32:I32"/>
+    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="C4:K4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C4:K4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2928,7 +3737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3174BC4-9706-45FC-9367-6AA2E623F9F9}">
   <dimension ref="A1:K65"/>
   <sheetViews>
@@ -2983,17 +3792,17 @@
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
@@ -3002,25 +3811,25 @@
       <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="15" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="K5" s="17"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
@@ -3029,7 +3838,7 @@
       <c r="B6" s="9">
         <v>100</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -3062,27 +3871,27 @@
       <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="16">
         <v>0.499</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="17">
         <f t="shared" ref="E7:E11" si="0">ABS(D7-$E$2)</f>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="16">
         <v>0.49480000000000002</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="17">
         <f t="shared" ref="G7:G11" si="1">ABS(F7-$E$2)</f>
         <v>5.1999999999999824E-3</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="16">
         <v>0.51229999999999998</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="17">
         <f t="shared" ref="I7:I11" si="2">ABS(H7-$E$2)</f>
         <v>1.2299999999999978E-2</v>
       </c>
@@ -3095,20 +3904,20 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="19">
         <v>0.49869999999999998</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="20">
         <f t="shared" si="0"/>
         <v>1.3000000000000234E-3</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="19">
         <v>0.49880000000000002</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="20">
         <f t="shared" si="1"/>
         <v>1.1999999999999789E-3</v>
       </c>
@@ -3119,36 +3928,36 @@
         <f t="shared" si="2"/>
         <v>4.9999999999994493E-4</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="19">
         <v>0.50190000000000001</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="20">
         <f t="shared" si="3"/>
         <v>1.9000000000000128E-3</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="16">
         <v>0.49070000000000003</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="17">
         <f t="shared" si="0"/>
         <v>9.299999999999975E-3</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="16">
         <v>0.50329999999999997</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="17">
         <f t="shared" si="1"/>
         <v>3.2999999999999696E-3</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="16">
         <v>0.49009999999999998</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="17">
         <f t="shared" si="2"/>
         <v>9.9000000000000199E-3</v>
       </c>
@@ -3161,7 +3970,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="13">
@@ -3171,36 +3980,36 @@
         <f t="shared" si="0"/>
         <v>2.9999999999996696E-4</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="19">
         <v>0.50680000000000003</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="20">
         <f t="shared" si="1"/>
         <v>6.8000000000000282E-3</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="19">
         <v>0.50590000000000002</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="20">
         <f t="shared" si="2"/>
         <v>5.9000000000000163E-3</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="19">
         <v>0.51029999999999998</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="20">
         <f t="shared" si="3"/>
         <v>1.0299999999999976E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="16">
         <v>0.50680000000000003</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="17">
         <f t="shared" si="0"/>
         <v>6.8000000000000282E-3</v>
       </c>
@@ -3211,17 +4020,17 @@
         <f t="shared" si="1"/>
         <v>5.4999999999999494E-3</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="16">
         <v>0.51319999999999999</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="17">
         <f t="shared" si="2"/>
         <v>1.319999999999999E-2</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="16">
         <v>0.51749999999999996</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="17">
         <f t="shared" si="3"/>
         <v>1.749999999999996E-2</v>
       </c>
@@ -3233,17 +4042,17 @@
       <c r="B13" s="9">
         <v>0</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="9" t="s">
@@ -3252,25 +4061,25 @@
       <c r="B14" s="9">
         <v>0</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="15" t="s">
+      <c r="E14" s="34"/>
+      <c r="F14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="15" t="s">
+      <c r="G14" s="34"/>
+      <c r="H14" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="15" t="s">
+      <c r="I14" s="34"/>
+      <c r="J14" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="K14" s="17"/>
+      <c r="K14" s="34"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="9" t="s">
@@ -3279,7 +4088,7 @@
       <c r="B15" s="9">
         <v>3</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
@@ -3489,15 +4298,15 @@
       <c r="B22" s="9">
         <v>0</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="9" t="s">
@@ -3506,21 +4315,21 @@
       <c r="B23" s="9">
         <v>2.5</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="15" t="s">
+      <c r="E23" s="34"/>
+      <c r="F23" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="15" t="s">
+      <c r="G23" s="34"/>
+      <c r="H23" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="17"/>
+      <c r="I23" s="34"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24" s="9" t="s">
@@ -3529,7 +4338,7 @@
       <c r="B24" s="9">
         <v>0.5</v>
       </c>
-      <c r="C24" s="19"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
@@ -3698,15 +4507,15 @@
       <c r="B31" s="9">
         <v>0</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="17"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="34"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A32" s="9" t="s">
@@ -3715,21 +4524,21 @@
       <c r="B32" s="9">
         <v>2</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="15" t="s">
+      <c r="E32" s="34"/>
+      <c r="F32" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="15" t="s">
+      <c r="G32" s="34"/>
+      <c r="H32" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I32" s="17"/>
+      <c r="I32" s="34"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A33" s="9" t="s">
@@ -3738,7 +4547,7 @@
       <c r="B33" s="9">
         <v>1</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
@@ -3907,15 +4716,15 @@
       <c r="B40" s="9">
         <v>0</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="17"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="34"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A41" s="9" t="s">
@@ -3924,21 +4733,21 @@
       <c r="B41" s="9">
         <v>1.5</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="15" t="s">
+      <c r="E41" s="34"/>
+      <c r="F41" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G41" s="17"/>
-      <c r="H41" s="15" t="s">
+      <c r="G41" s="34"/>
+      <c r="H41" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I41" s="17"/>
+      <c r="I41" s="34"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A42" s="9" t="s">
@@ -3947,7 +4756,7 @@
       <c r="B42" s="9">
         <v>1.5</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="36"/>
       <c r="D42" s="1" t="s">
         <v>10</v>
       </c>
@@ -4116,15 +4925,15 @@
       <c r="B49" s="9">
         <v>0</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="17"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="34"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A50" s="9" t="s">
@@ -4133,21 +4942,21 @@
       <c r="B50" s="9">
         <v>1</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="17"/>
-      <c r="F50" s="15" t="s">
+      <c r="E50" s="34"/>
+      <c r="F50" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G50" s="17"/>
-      <c r="H50" s="15" t="s">
+      <c r="G50" s="34"/>
+      <c r="H50" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I50" s="17"/>
+      <c r="I50" s="34"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A51" s="9" t="s">
@@ -4156,7 +4965,7 @@
       <c r="B51" s="9">
         <v>2</v>
       </c>
-      <c r="C51" s="19"/>
+      <c r="C51" s="36"/>
       <c r="D51" s="1" t="s">
         <v>10</v>
       </c>
@@ -4325,15 +5134,15 @@
       <c r="B58" s="9">
         <v>0</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="17"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A59" s="9" t="s">
@@ -4342,21 +5151,21 @@
       <c r="B59" s="9">
         <v>0.5</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="15" t="s">
+      <c r="E59" s="34"/>
+      <c r="F59" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="15" t="s">
+      <c r="G59" s="34"/>
+      <c r="H59" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I59" s="17"/>
+      <c r="I59" s="34"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A60" s="9" t="s">
@@ -4365,7 +5174,7 @@
       <c r="B60" s="9">
         <v>2.5</v>
       </c>
-      <c r="C60" s="19"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="1" t="s">
         <v>10</v>
       </c>
@@ -4529,28 +5338,28 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="C13:K13"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="C40:I40"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="D41:E41"/>
@@ -4573,7 +5382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6172D4-1552-4A91-BEBB-E75DBE13E8F4}">
   <dimension ref="A1:I20"/>
   <sheetViews>
@@ -4628,15 +5437,15 @@
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
@@ -4645,21 +5454,21 @@
       <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="17"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
@@ -4668,7 +5477,7 @@
       <c r="B6" s="9">
         <v>100</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -4831,15 +5640,15 @@
       <c r="B13" s="9">
         <v>0</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" s="9" t="s">
@@ -4848,21 +5657,21 @@
       <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="15" t="s">
+      <c r="E14" s="34"/>
+      <c r="F14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="15" t="s">
+      <c r="G14" s="34"/>
+      <c r="H14" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="17"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="9" t="s">
@@ -4871,7 +5680,7 @@
       <c r="B15" s="9">
         <v>100</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
@@ -5046,7 +5855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694FA8BF-FDF9-4164-B4EA-D9FA0E639984}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -5101,15 +5910,15 @@
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
@@ -5118,21 +5927,21 @@
       <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="17"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
@@ -5141,7 +5950,7 @@
       <c r="B6" s="9">
         <v>100</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -5304,15 +6113,15 @@
       <c r="B13" s="9">
         <v>0</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" s="9" t="s">
@@ -5321,21 +6130,21 @@
       <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="15" t="s">
+      <c r="E14" s="34"/>
+      <c r="F14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="15" t="s">
+      <c r="G14" s="34"/>
+      <c r="H14" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="17"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="9" t="s">
@@ -5344,7 +6153,7 @@
       <c r="B15" s="9">
         <v>0.4</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
@@ -5516,15 +6325,15 @@
       <c r="B22" s="9">
         <v>0</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" s="9" t="s">
@@ -5533,21 +6342,21 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="15" t="s">
+      <c r="E23" s="34"/>
+      <c r="F23" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="15" t="s">
+      <c r="G23" s="34"/>
+      <c r="H23" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="17"/>
+      <c r="I23" s="34"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" s="9" t="s">
@@ -5556,7 +6365,7 @@
       <c r="B24" s="9">
         <v>100</v>
       </c>
-      <c r="C24" s="19"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
@@ -5736,7 +6545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{008E6B94-C183-4448-A9CE-DA3924432B8F}">
   <dimension ref="A1:K38"/>
   <sheetViews>
@@ -5791,17 +6600,17 @@
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
@@ -5810,25 +6619,25 @@
       <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="34"/>
+      <c r="H5" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="15" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="17"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
@@ -5837,7 +6646,7 @@
       <c r="B6" s="9">
         <v>100</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -6041,17 +6850,17 @@
       <c r="B13" s="9">
         <v>0</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="9" t="s">
@@ -6060,25 +6869,25 @@
       <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="15" t="s">
+      <c r="E14" s="34"/>
+      <c r="F14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="15" t="s">
+      <c r="G14" s="34"/>
+      <c r="H14" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="15" t="s">
+      <c r="I14" s="34"/>
+      <c r="J14" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="17"/>
+      <c r="K14" s="34"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="9" t="s">
@@ -6087,7 +6896,7 @@
       <c r="B15" s="9">
         <v>100</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
@@ -6291,17 +7100,17 @@
       <c r="B22" s="9">
         <v>0</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="17"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="34"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="9" t="s">
@@ -6310,25 +7119,25 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="15" t="s">
+      <c r="E23" s="34"/>
+      <c r="F23" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="15" t="s">
+      <c r="G23" s="34"/>
+      <c r="H23" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="15" t="s">
+      <c r="I23" s="34"/>
+      <c r="J23" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="17"/>
+      <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24" s="9" t="s">
@@ -6337,7 +7146,7 @@
       <c r="B24" s="9">
         <v>100</v>
       </c>
-      <c r="C24" s="19"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
@@ -6541,17 +7350,17 @@
       <c r="B31" s="9">
         <v>0</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="17"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="34"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A32" s="9" t="s">
@@ -6560,25 +7369,25 @@
       <c r="B32" s="9">
         <v>3</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="15" t="s">
+      <c r="E32" s="34"/>
+      <c r="F32" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="15" t="s">
+      <c r="G32" s="34"/>
+      <c r="H32" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="17"/>
-      <c r="J32" s="15" t="s">
+      <c r="I32" s="34"/>
+      <c r="J32" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="17"/>
+      <c r="K32" s="34"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A33" s="9" t="s">
@@ -6587,7 +7396,7 @@
       <c r="B33" s="9">
         <v>100</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>